<commit_message>
Committed with updated data
</commit_message>
<xml_diff>
--- a/City Data.xlsx
+++ b/City Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\ukraine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23C3B9A9-F2EC-49B6-BF94-B017BDE438E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0EF6D-B461-4C41-8F3A-7FB90EB95189}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3C8E989B-EBB0-44F1-B85E-44A0B627C20D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="28">
   <si>
     <t>City</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>2019 Oblast HDI</t>
+  </si>
+  <si>
+    <t>Total Ukr Cases</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB877DDD-97FB-45B4-87B0-3782CBA074C1}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,9 +483,10 @@
     <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,8 +511,11 @@
       <c r="H1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -533,8 +540,11 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <v>323448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -559,8 +569,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>323448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -585,8 +598,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <v>323448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -611,8 +627,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <v>323448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -637,8 +656,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <v>241629</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -663,8 +685,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <v>241629</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -689,8 +714,11 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8">
+        <v>241629</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -715,8 +743,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9">
+        <v>241629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -741,8 +772,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <v>311484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -767,8 +801,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <v>311484</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -793,8 +830,11 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>311484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -819,8 +859,11 @@
       <c r="H13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <v>311484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -845,8 +888,11 @@
       <c r="H14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14">
+        <v>371768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -871,8 +917,11 @@
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15">
+        <v>371768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -897,8 +946,11 @@
       <c r="H16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>371768</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -923,8 +975,11 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <v>371768</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -949,8 +1004,11 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <v>344581</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -975,8 +1033,11 @@
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <v>344581</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1001,8 +1062,11 @@
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <v>344581</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1027,8 +1091,11 @@
       <c r="H21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <v>344581</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1053,8 +1120,11 @@
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22">
+        <v>369162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1079,8 +1149,11 @@
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23">
+        <v>369162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1105,8 +1178,11 @@
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <v>369162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1131,8 +1207,11 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <v>369162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1157,8 +1236,11 @@
       <c r="H26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26">
+        <v>411341</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1183,8 +1265,11 @@
       <c r="H27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27">
+        <v>411341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1209,8 +1294,11 @@
       <c r="H28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28">
+        <v>411341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1235,8 +1323,11 @@
       <c r="H29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>411341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1261,8 +1352,11 @@
       <c r="H30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>416328</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1287,8 +1381,11 @@
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31">
+        <v>416328</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1313,8 +1410,11 @@
       <c r="H32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32">
+        <v>416328</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1339,8 +1439,11 @@
       <c r="H33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33">
+        <v>416328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1365,8 +1468,11 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34">
+        <v>406495</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1391,8 +1497,11 @@
       <c r="H35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35">
+        <v>406495</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -1417,8 +1526,11 @@
       <c r="H36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36">
+        <v>406495</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1443,8 +1555,11 @@
       <c r="H37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37">
+        <v>406495</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1469,8 +1584,11 @@
       <c r="H38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38">
+        <v>407589</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -1495,8 +1613,11 @@
       <c r="H39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39">
+        <v>407589</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -1521,8 +1642,11 @@
       <c r="H40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I40">
+        <v>407589</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -1547,8 +1671,11 @@
       <c r="H41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I41">
+        <v>407589</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -1570,8 +1697,11 @@
       <c r="H42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I42">
+        <v>404793</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -1593,8 +1723,11 @@
       <c r="H43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I43">
+        <v>404793</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -1616,8 +1749,11 @@
       <c r="H44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I44">
+        <v>404793</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -1639,8 +1775,11 @@
       <c r="H45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I45">
+        <v>404793</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -1665,8 +1804,11 @@
       <c r="H46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I46">
+        <v>392189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1691,8 +1833,11 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I47">
+        <v>392189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -1717,8 +1862,11 @@
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48">
+        <v>392189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -1742,6 +1890,9 @@
       </c>
       <c r="H49">
         <v>0</v>
+      </c>
+      <c r="I49">
+        <v>392189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit with included Kramatorsk
</commit_message>
<xml_diff>
--- a/City Data.xlsx
+++ b/City Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\ukraine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0EF6D-B461-4C41-8F3A-7FB90EB95189}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0B3233-8AD2-4E1E-A4D2-ADF0CBBCA785}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3C8E989B-EBB0-44F1-B85E-44A0B627C20D}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>Donetsk</t>
   </si>
   <si>
-    <t>Oblast Center</t>
-  </si>
-  <si>
     <t>2020 City Population</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Total Ukr Cases</t>
+  </si>
+  <si>
+    <t>Not Oblast Center</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,16 +503,16 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -538,7 +538,7 @@
         <v>1017699</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>323448</v>
@@ -567,7 +567,7 @@
         <v>1017699</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>323448</v>
@@ -596,7 +596,7 @@
         <v>1017699</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>323448</v>
@@ -625,7 +625,7 @@
         <v>1017699</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>323448</v>
@@ -654,7 +654,7 @@
         <v>48674</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>241629</v>
@@ -683,7 +683,7 @@
         <v>48674</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>241629</v>
@@ -712,7 +712,7 @@
         <v>48674</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>241629</v>
@@ -741,7 +741,7 @@
         <v>48674</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>241629</v>
@@ -770,7 +770,7 @@
         <v>286958</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>311484</v>
@@ -799,7 +799,7 @@
         <v>286958</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <v>311484</v>
@@ -828,7 +828,7 @@
         <v>286958</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>311484</v>
@@ -857,7 +857,7 @@
         <v>286958</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>311484</v>
@@ -886,7 +886,7 @@
         <v>724314</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>371768</v>
@@ -915,7 +915,7 @@
         <v>724314</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <v>371768</v>
@@ -944,7 +944,7 @@
         <v>724314</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>371768</v>
@@ -973,7 +973,7 @@
         <v>724314</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <v>371768</v>
@@ -1002,7 +1002,7 @@
         <v>237686</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>344581</v>
@@ -1031,7 +1031,7 @@
         <v>237686</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <v>344581</v>
@@ -1060,7 +1060,7 @@
         <v>237686</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>344581</v>
@@ -1089,7 +1089,7 @@
         <v>237686</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>344581</v>
@@ -1118,7 +1118,7 @@
         <v>75396</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>369162</v>
@@ -1147,7 +1147,7 @@
         <v>75396</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>369162</v>
@@ -1176,7 +1176,7 @@
         <v>75396</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <v>369162</v>
@@ -1205,7 +1205,7 @@
         <v>75396</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>369162</v>
@@ -1234,7 +1234,7 @@
         <v>2967360</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
         <v>411341</v>
@@ -1263,7 +1263,7 @@
         <v>2967360</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>411341</v>
@@ -1292,7 +1292,7 @@
         <v>2967360</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <v>411341</v>
@@ -1321,7 +1321,7 @@
         <v>2967360</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29">
         <v>411341</v>
@@ -1350,7 +1350,7 @@
         <v>209238</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>416328</v>
@@ -1379,7 +1379,7 @@
         <v>209238</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>416328</v>
@@ -1408,7 +1408,7 @@
         <v>209238</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <v>416328</v>
@@ -1437,7 +1437,7 @@
         <v>209238</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>416328</v>
@@ -1466,7 +1466,7 @@
         <v>45032</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <v>406495</v>
@@ -1495,7 +1495,7 @@
         <v>45032</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>406495</v>
@@ -1524,7 +1524,7 @@
         <v>45032</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <v>406495</v>
@@ -1553,7 +1553,7 @@
         <v>45032</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>406495</v>
@@ -1582,7 +1582,7 @@
         <v>1443207</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
         <v>407589</v>
@@ -1611,7 +1611,7 @@
         <v>1443207</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39">
         <v>407589</v>
@@ -1640,7 +1640,7 @@
         <v>1443207</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
         <v>407589</v>
@@ -1669,7 +1669,7 @@
         <v>1443207</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41">
         <v>407589</v>
@@ -1695,7 +1695,7 @@
         <v>152120</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42">
         <v>404793</v>
@@ -1721,7 +1721,7 @@
         <v>152120</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <v>404793</v>
@@ -1747,7 +1747,7 @@
         <v>152120</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44">
         <v>404793</v>
@@ -1773,7 +1773,7 @@
         <v>152120</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <v>404793</v>
@@ -1802,7 +1802,7 @@
         <v>46653</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <v>392189</v>
@@ -1831,7 +1831,7 @@
         <v>46653</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47">
         <v>392189</v>
@@ -1860,7 +1860,7 @@
         <v>46653</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <v>392189</v>
@@ -1889,7 +1889,7 @@
         <v>46653</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49">
         <v>392189</v>

</xml_diff>

<commit_message>
Commit with updated results
</commit_message>
<xml_diff>
--- a/City Data.xlsx
+++ b/City Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\ukraine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0B3233-8AD2-4E1E-A4D2-ADF0CBBCA785}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090321CA-738B-4C00-9A07-4C9067238EFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3C8E989B-EBB0-44F1-B85E-44A0B627C20D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="34">
   <si>
     <t>City</t>
   </si>
@@ -118,6 +118,24 @@
   </si>
   <si>
     <t>Not Oblast Center</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>2001 Pct Russian</t>
   </si>
 </sst>
 </file>
@@ -469,24 +487,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB877DDD-97FB-45B4-87B0-3782CBA074C1}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,28 +512,34 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -523,28 +547,34 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>9.4076655099999993</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>54</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.65900000000000003</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1017699</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>323448</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>64.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -552,28 +582,34 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>8.8850174200000005</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>51</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.65900000000000003</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1017699</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>323448</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>64.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -581,28 +617,34 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>25.958188</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>149</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.65900000000000003</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1017699</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>323448</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>64.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -610,28 +652,34 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>55.749129000000003</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>320</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.65900000000000003</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1017699</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>323448</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>64.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -639,28 +687,34 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>21.052631999999999</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>36</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.65900000000000003</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>48674</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>241629</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>54.52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -668,28 +722,34 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>21.052631999999999</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>36</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.65900000000000003</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>48674</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>241629</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>54.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -697,28 +757,34 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>23.976607999999999</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>41</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.65900000000000003</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>48674</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>241629</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>54.52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -726,28 +792,34 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>33.918129</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>58</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.65900000000000003</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>48674</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>241629</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>54.52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -755,28 +827,34 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>8.3333333300000003</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>43</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.61499999999999999</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>286958</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>311484</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K10">
+        <v>45.34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -784,28 +862,34 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>8.1395348799999994</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>42</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.61499999999999999</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>286958</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
       <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>311484</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <v>45.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -813,28 +897,34 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>26.356589100000001</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>136</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>0.61499999999999999</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>286958</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>311484</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K12">
+        <v>45.34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -842,28 +932,34 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>57.170542599999997</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>295</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>0.61499999999999999</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>286958</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
       <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
         <v>311484</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>45.34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -871,28 +967,34 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>1.2605042</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>6</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>724314</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
       <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
         <v>371768</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K14">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -900,28 +1002,34 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0.84033612999999996</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>4</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>724314</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
       <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
         <v>371768</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K15">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -929,28 +1037,34 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>15.1260504</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>72</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>724314</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
         <v>371768</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -958,28 +1072,34 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>82.773109199999993</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>394</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>724314</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
       <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
         <v>371768</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K17">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -987,28 +1107,34 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
         <v>15</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>1.28354726</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>11</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>0.68500000000000005</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>237686</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
       <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>344581</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K18">
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1016,28 +1142,34 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>1.6336056000000001</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>14</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>0.68500000000000005</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>237686</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
       <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
         <v>344581</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K19">
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1045,28 +1177,34 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
         <v>17</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>17.852975499999999</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>153</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>0.68500000000000005</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>237686</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
       <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
         <v>344581</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K20">
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1074,28 +1212,34 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>79.229872</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>679</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>0.68500000000000005</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>237686</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
       <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
         <v>344581</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K21">
+        <v>6.79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1103,28 +1247,34 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
         <v>15</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>2.8634361199999998</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>13</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>75396</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>1</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>369162</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K22">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1132,28 +1282,34 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>1.76211454</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>8</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>75396</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>1</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>369162</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K23">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1161,28 +1317,34 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
         <v>17</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>21.8061674</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>99</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>75396</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>1</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>369162</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K24">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1190,28 +1352,34 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
         <v>18</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>73.568281900000002</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>334</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>75396</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>1</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>369162</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K25">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1219,28 +1387,34 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
         <v>15</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>1.5810276700000001</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>8</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>0.874</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>2967360</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
       <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
         <v>411341</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K26">
+        <v>25.27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1248,28 +1422,34 @@
         <v>21</v>
       </c>
       <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
         <v>16</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>0.59288538000000002</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>3</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>0.874</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>2967360</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
       <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
         <v>411341</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K27">
+        <v>25.27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1277,28 +1457,34 @@
         <v>21</v>
       </c>
       <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
         <v>17</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>10.474308300000001</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>53</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>0.874</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>2967360</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
       <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
         <v>411341</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K28">
+        <v>25.27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1306,28 +1492,34 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
         <v>18</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>87.351778699999997</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>442</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>0.874</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>2967360</v>
       </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
       <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>411341</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K29">
+        <v>25.27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1335,28 +1527,34 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
         <v>15</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>1.3824884799999999</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>9</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>209238</v>
       </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
       <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
         <v>416328</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K30">
+        <v>12.31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1364,28 +1562,34 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
         <v>16</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>1.07526882</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>7</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>209238</v>
       </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
       <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
         <v>416328</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K31">
+        <v>12.31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1393,28 +1597,34 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
         <v>17</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>15.053763399999999</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>98</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>209238</v>
       </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
       <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
         <v>416328</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K32">
+        <v>12.31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1422,28 +1632,34 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
         <v>18</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>82.488479299999995</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>537</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>209238</v>
       </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
       <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
         <v>416328</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K33">
+        <v>12.31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1451,28 +1667,34 @@
         <v>22</v>
       </c>
       <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
         <v>15</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>8.9385474899999995</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>48</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>0.65</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>45032</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>1</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>406495</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K34">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1480,28 +1702,34 @@
         <v>22</v>
       </c>
       <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
         <v>16</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>6.1452514000000003</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>33</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>0.65</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>45032</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>1</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>406495</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K35">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -1509,28 +1737,34 @@
         <v>22</v>
       </c>
       <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
         <v>17</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>22.9050279</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>123</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>0.65</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>45032</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>1</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>406495</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K36">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1538,28 +1772,34 @@
         <v>22</v>
       </c>
       <c r="C37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>62.011173200000002</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>333</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>0.65</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>45032</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>1</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>406495</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K37">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1567,28 +1807,34 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>4.2830539999999999</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>23</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>1443207</v>
       </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
       <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
         <v>407589</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K38">
+        <v>65.86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -1596,28 +1842,34 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" t="s">
         <v>16</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>4.0968342599999996</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>22</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>1443207</v>
       </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
       <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
         <v>407589</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K39">
+        <v>65.86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -1625,28 +1877,34 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s">
         <v>17</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>24.7672253</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>133</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>1443207</v>
       </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
       <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
         <v>407589</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K40">
+        <v>65.86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -1654,28 +1912,34 @@
         <v>12</v>
       </c>
       <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" t="s">
         <v>18</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>70.577281200000002</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>379</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>1443207</v>
       </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
       <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
         <v>407589</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K41">
+        <v>65.86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -1683,25 +1947,31 @@
         <v>23</v>
       </c>
       <c r="C42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" t="s">
         <v>15</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>2.0737327200000002</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>9</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>152120</v>
       </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
       <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
         <v>404793</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K42">
+        <v>67.87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -1709,25 +1979,31 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
         <v>16</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>2.7649769599999998</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>12</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>152120</v>
       </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
       <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
         <v>404793</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K43">
+        <v>67.87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -1735,25 +2011,31 @@
         <v>23</v>
       </c>
       <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" t="s">
         <v>17</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>17.050691199999999</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>74</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>152120</v>
       </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
       <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
         <v>404793</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K44">
+        <v>67.87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -1761,25 +2043,31 @@
         <v>23</v>
       </c>
       <c r="C45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" t="s">
         <v>18</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>78.110599100000002</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>339</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>152120</v>
       </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
       <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
         <v>404793</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K45">
+        <v>67.87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -1787,28 +2075,34 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" t="s">
         <v>15</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>5.8951965099999999</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>27</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>46653</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>1</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>392189</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K46">
+        <v>23.77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -1816,28 +2110,34 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" t="s">
         <v>16</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>5.8951965099999999</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>27</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>46653</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>1</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>392189</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K47">
+        <v>23.77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -1845,28 +2145,34 @@
         <v>12</v>
       </c>
       <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
         <v>17</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>22.489083000000001</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>103</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>46653</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>1</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>392189</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K48">
+        <v>23.77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -1874,25 +2180,31 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" t="s">
         <v>18</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>65.720523999999997</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>301</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>46653</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>1</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>392189</v>
+      </c>
+      <c r="K49">
+        <v>23.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited city data, added a couple of graphs
</commit_message>
<xml_diff>
--- a/City Data.xlsx
+++ b/City Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\ukraine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B928071F-5830-4FF1-93C1-9C518E89908F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625D328C-3ACC-436F-B0D8-E358E42A7983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3C8E989B-EBB0-44F1-B85E-44A0B627C20D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="43">
   <si>
     <t>City</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>Red Zone</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB877DDD-97FB-45B4-87B0-3782CBA074C1}">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,7 +531,7 @@
     <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +580,11 @@
       <c r="P1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -627,8 +633,11 @@
       <c r="P2">
         <v>12.12</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -677,8 +686,11 @@
       <c r="P3">
         <v>12.12</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -727,8 +739,11 @@
       <c r="P4">
         <v>12.12</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -777,8 +792,11 @@
       <c r="P5">
         <v>12.12</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -827,8 +845,11 @@
       <c r="P6">
         <v>7.03</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -877,8 +898,11 @@
       <c r="P7">
         <v>7.03</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -927,8 +951,11 @@
       <c r="P8">
         <v>7.03</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -977,8 +1004,11 @@
       <c r="P9">
         <v>7.03</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1027,8 +1057,11 @@
       <c r="P10">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1077,8 +1110,11 @@
       <c r="P11">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1127,8 +1163,11 @@
       <c r="P12">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1177,8 +1216,11 @@
       <c r="P13">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1227,8 +1269,11 @@
       <c r="P14">
         <v>42.72</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1277,8 +1322,11 @@
       <c r="P15">
         <v>42.72</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1327,8 +1375,11 @@
       <c r="P16">
         <v>42.72</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1377,8 +1428,11 @@
       <c r="P17">
         <v>42.72</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1427,8 +1481,11 @@
       <c r="P18">
         <v>26.79</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1477,8 +1534,11 @@
       <c r="P19">
         <v>26.79</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1527,8 +1587,11 @@
       <c r="P20">
         <v>26.79</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1577,8 +1640,11 @@
       <c r="P21">
         <v>26.79</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1627,8 +1693,11 @@
       <c r="P22">
         <v>30.24</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1677,8 +1746,11 @@
       <c r="P23">
         <v>30.24</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1727,8 +1799,11 @@
       <c r="P24">
         <v>30.24</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1777,8 +1852,11 @@
       <c r="P25">
         <v>30.24</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1827,8 +1905,11 @@
       <c r="P26">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1877,8 +1958,11 @@
       <c r="P27">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1927,8 +2011,11 @@
       <c r="P28">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1977,8 +2064,11 @@
       <c r="P29">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -2027,8 +2117,11 @@
       <c r="P30">
         <v>15.29</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2077,8 +2170,11 @@
       <c r="P31">
         <v>15.29</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2127,8 +2223,11 @@
       <c r="P32">
         <v>15.29</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -2177,8 +2276,11 @@
       <c r="P33">
         <v>15.29</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2227,8 +2329,11 @@
       <c r="P34">
         <v>10.35</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -2277,8 +2382,11 @@
       <c r="P35">
         <v>10.35</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2327,8 +2435,11 @@
       <c r="P36">
         <v>10.35</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2377,8 +2488,11 @@
       <c r="P37">
         <v>10.35</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2427,8 +2541,11 @@
       <c r="P38">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2477,8 +2594,11 @@
       <c r="P39">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2527,8 +2647,11 @@
       <c r="P40">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2577,8 +2700,11 @@
       <c r="P41">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2624,8 +2750,11 @@
       <c r="P42">
         <v>13.04</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2671,8 +2800,11 @@
       <c r="P43">
         <v>13.04</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2718,8 +2850,11 @@
       <c r="P44">
         <v>13.04</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2765,8 +2900,11 @@
       <c r="P45">
         <v>13.04</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2815,8 +2953,11 @@
       <c r="P46">
         <v>6.83</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2865,8 +3006,11 @@
       <c r="P47">
         <v>6.83</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -2915,8 +3059,11 @@
       <c r="P48">
         <v>6.83</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -2965,8 +3112,12 @@
       <c r="P49">
         <v>6.83</v>
       </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>